<commit_message>
scheduler added and subsidies table fix
</commit_message>
<xml_diff>
--- a/subsid.xlsx
+++ b/subsid.xlsx
@@ -441,12 +441,12 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>МО</t>
+          <t>Муниципалитет</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Н.п.</t>
+          <t>Населенный пункт</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -689,10 +689,26 @@
           <t>Хомутово д.</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr"/>
-      <c r="F7" t="inlineStr"/>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="inlineStr"/>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -1096,7 +1112,7 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1113,14 +1129,30 @@
           <t>Бобровка с.</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr"/>
-      <c r="F18" t="inlineStr"/>
-      <c r="G18" t="inlineStr"/>
-      <c r="H18" t="inlineStr"/>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1137,14 +1169,30 @@
           <t>Михайловка с.</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr"/>
-      <c r="F19" t="inlineStr"/>
-      <c r="G19" t="inlineStr"/>
-      <c r="H19" t="inlineStr"/>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1161,14 +1209,30 @@
           <t>Антропово с.</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr"/>
-      <c r="F20" t="inlineStr"/>
-      <c r="G20" t="inlineStr"/>
-      <c r="H20" t="inlineStr"/>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1185,14 +1249,30 @@
           <t>Костеньки д.</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr"/>
-      <c r="F21" t="inlineStr"/>
-      <c r="G21" t="inlineStr"/>
-      <c r="H21" t="inlineStr"/>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -1209,14 +1289,30 @@
           <t>Завировка д.</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr"/>
-      <c r="F22" t="inlineStr"/>
-      <c r="G22" t="inlineStr"/>
-      <c r="H22" t="inlineStr"/>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -1233,14 +1329,30 @@
           <t>Бакчет с.</t>
         </is>
       </c>
-      <c r="E23" t="inlineStr"/>
-      <c r="F23" t="inlineStr"/>
-      <c r="G23" t="inlineStr"/>
-      <c r="H23" t="inlineStr"/>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -1257,10 +1369,26 @@
           <t>Красный Хутор п.</t>
         </is>
       </c>
-      <c r="E24" t="inlineStr"/>
-      <c r="F24" t="inlineStr"/>
-      <c r="G24" t="inlineStr"/>
-      <c r="H24" t="inlineStr"/>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>